<commit_message>
Letzte Korrekturen. Abnahme Zip geschnürrt.
</commit_message>
<xml_diff>
--- a/Praktikum 2/Mängelliste_Team2.1.xlsx
+++ b/Praktikum 2/Mängelliste_Team2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\franek\Documents\Programming\Java\SE1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\HAW\SE\SEP\Praktikum 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="113">
   <si>
     <t>Gutachter</t>
   </si>
@@ -248,9 +248,6 @@
   </si>
   <si>
     <t>Cloud ins Glossar aufnehmen.</t>
-  </si>
-  <si>
-    <t>TODO</t>
   </si>
   <si>
     <t>Stimmt</t>
@@ -287,9 +284,6 @@
     </r>
   </si>
   <si>
-    <t>Kudenservice?         Warum ist Kundenservice schlechter als ein Servicetechniker</t>
-  </si>
-  <si>
     <t>Verbesserung der Interessenbeschreibung</t>
   </si>
   <si>
@@ -371,9 +365,6 @@
     <t>Stakeholder wurde auf Dyson geändert</t>
   </si>
   <si>
-    <t>TÜV ist staatliche Qualitätssicherung, an die sich gehaltenw erden muss!</t>
-  </si>
-  <si>
     <t>Es ist wohl besser für uns, wenn wir die entfernen. So muss nicht auch hie rnoch eine Versionsnumme rmitgeschleppt werden. Zumal ja nur das akutelle interessiert.</t>
   </si>
   <si>
@@ -384,6 +375,18 @@
   </si>
   <si>
     <t>Karte muss vorhanden sein ja. Aber der Roboter soll auch auf freiem Feld einen Saugvorgang fortsetzen können FALSCH, das ist dann schon im Aklternativszenario beschrieben!</t>
+  </si>
+  <si>
+    <t>TÜV ist staatliche Qualitätssicherung, an die sich gehalten werden muss!</t>
+  </si>
+  <si>
+    <t>Kudenservice?         Warum ist Kundenservice schlechter als ein Servicetechniker?</t>
+  </si>
+  <si>
+    <t>Akteur Roboter hinzugefügt und Hauptszenario mehr auf akteure angepasst.</t>
+  </si>
+  <si>
+    <t>Karte hinzugefügt</t>
   </si>
 </sst>
 </file>
@@ -749,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,7 +761,7 @@
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="105.5703125" customWidth="1"/>
+    <col min="9" max="9" width="143.5703125" customWidth="1"/>
     <col min="10" max="10" width="103.85546875" customWidth="1"/>
     <col min="11" max="11" width="80.7109375" customWidth="1"/>
     <col min="12" max="12" width="48.5703125" customWidth="1"/>
@@ -797,7 +800,7 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -820,16 +823,16 @@
         <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -854,7 +857,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
       <c r="I4" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J4" s="5"/>
     </row>
@@ -878,16 +881,16 @@
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -913,10 +916,10 @@
         <v>71</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>73</v>
@@ -942,14 +945,14 @@
         <v>2</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1006,7 +1009,7 @@
         <v>72</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J9" s="5"/>
     </row>
@@ -1033,10 +1036,10 @@
         <v>71</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J10" s="5"/>
     </row>
@@ -1060,16 +1063,16 @@
         <v>2</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I11" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1095,10 +1098,10 @@
         <v>71</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J12" s="5"/>
     </row>
@@ -1113,7 +1116,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -1125,10 +1128,10 @@
         <v>71</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -1155,13 +1158,13 @@
         <v>71</v>
       </c>
       <c r="H14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="J14" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1184,16 +1187,16 @@
         <v>1</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1219,12 +1222,14 @@
         <v>71</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="J16" s="5"/>
+        <v>107</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -1249,12 +1254,14 @@
         <v>71</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="J17" s="5"/>
+        <v>108</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1276,14 +1283,14 @@
         <v>4</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1306,16 +1313,16 @@
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1338,14 +1345,14 @@
         <v>1</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1368,14 +1375,14 @@
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1398,10 +1405,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -1426,14 +1433,14 @@
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1456,14 +1463,14 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1486,13 +1493,13 @@
         <v>2</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J25" s="5"/>
     </row>
@@ -1516,16 +1523,16 @@
         <v>2</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1548,14 +1555,14 @@
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1578,14 +1585,14 @@
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1608,10 +1615,10 @@
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -1660,10 +1667,10 @@
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -1688,10 +1695,10 @@
         <v>2</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -1716,10 +1723,10 @@
         <v>2</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -1744,16 +1751,16 @@
         <v>3</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1773,14 +1780,14 @@
         <v>3</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>